<commit_message>
update elec/ARpUIIRC (take out US values)
</commit_message>
<xml_diff>
--- a/InputData/elec/ARpUIiRC/Ann Ret per Unit Inc in Relative Cost.xlsx
+++ b/InputData/elec/ARpUIiRC/Ann Ret per Unit Inc in Relative Cost.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MeganM\Documents\eps-us\InputData\elec\ARpUIiRC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivia\Documents\EPS_Models by Region\South Korea\eps-southkorea\InputData\elec\ARpUIiRC\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C97700-03AB-49FC-BF01-F57F9354B50D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="21075" windowHeight="9030" tabRatio="606"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="14020" tabRatio="606" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -26,7 +27,18 @@
     <definedName name="dollars_2020_2012">[1]About!$A$103</definedName>
     <definedName name="nonlignite_multiplier">'[1]Hard Coal and Lig Multipliers'!$N$16</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -650,7 +662,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -831,16 +843,16 @@
     </xf>
   </cellXfs>
   <cellStyles count="10">
-    <cellStyle name="Body: normal cell" xfId="7"/>
-    <cellStyle name="Font: Calibri, 9pt regular" xfId="3"/>
-    <cellStyle name="Footnotes: top row" xfId="8"/>
-    <cellStyle name="Header: bottom row" xfId="4"/>
+    <cellStyle name="Body: normal cell" xfId="7" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Font: Calibri, 9pt regular" xfId="3" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Footnotes: top row" xfId="8" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Header: bottom row" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2"/>
-    <cellStyle name="Parent row" xfId="6"/>
+    <cellStyle name="Normal 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="Parent row" xfId="6" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="Table title" xfId="5"/>
+    <cellStyle name="Table title" xfId="5" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3440,7 +3452,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3470,7 +3488,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -3709,6 +3733,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -3744,6 +3785,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -3919,21 +3977,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A55" sqref="A55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -3946,30 +4004,30 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="3">
         <v>2021</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
       <c r="B6" s="13" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B9" s="12" t="s">
         <v>62</v>
       </c>
@@ -3979,212 +4037,212 @@
       <c r="F9" s="10"/>
       <c r="G9" s="10"/>
     </row>
-    <row r="10" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:7" s="16" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="17" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>0.9</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>59</v>
       </c>
@@ -4196,36 +4254,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AH37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:34" s="11" customFormat="1" ht="114" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:34" s="11" customFormat="1" ht="116" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>128</v>
       </c>
@@ -4329,7 +4387,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2050</v>
       </c>
@@ -4433,7 +4491,7 @@
         <v>1858.9445800000001</v>
       </c>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2049</v>
       </c>
@@ -4537,7 +4595,7 @@
         <v>1827.3076169999999</v>
       </c>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2048</v>
       </c>
@@ -4641,7 +4699,7 @@
         <v>1786.3354489999999</v>
       </c>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2047</v>
       </c>
@@ -4745,7 +4803,7 @@
         <v>1752.4071039999999</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2046</v>
       </c>
@@ -4849,7 +4907,7 @@
         <v>1720.7452390000001</v>
       </c>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2045</v>
       </c>
@@ -4953,7 +5011,7 @@
         <v>1691.0301509999999</v>
       </c>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2044</v>
       </c>
@@ -5057,7 +5115,7 @@
         <v>1662.8668210000001</v>
       </c>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2043</v>
       </c>
@@ -5161,7 +5219,7 @@
         <v>1628.2060550000001</v>
       </c>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2042</v>
       </c>
@@ -5265,7 +5323,7 @@
         <v>1600.3344729999999</v>
       </c>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2041</v>
       </c>
@@ -5369,7 +5427,7 @@
         <v>1578.294312</v>
       </c>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2040</v>
       </c>
@@ -5473,7 +5531,7 @@
         <v>1558.4305420000001</v>
       </c>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2039</v>
       </c>
@@ -5577,7 +5635,7 @@
         <v>1529.5474850000001</v>
       </c>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2038</v>
       </c>
@@ -5681,7 +5739,7 @@
         <v>1505.713745</v>
       </c>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2037</v>
       </c>
@@ -5785,7 +5843,7 @@
         <v>1485.511841</v>
       </c>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2036</v>
       </c>
@@ -5889,7 +5947,7 @@
         <v>1466.6623540000001</v>
       </c>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2035</v>
       </c>
@@ -5993,7 +6051,7 @@
         <v>1446.490601</v>
       </c>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2034</v>
       </c>
@@ -6097,7 +6155,7 @@
         <v>1417.6995850000001</v>
       </c>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2033</v>
       </c>
@@ -6201,7 +6259,7 @@
         <v>1394.9499510000001</v>
       </c>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2032</v>
       </c>
@@ -6305,7 +6363,7 @@
         <v>1380.4626459999999</v>
       </c>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2031</v>
       </c>
@@ -6409,7 +6467,7 @@
         <v>1364.06665</v>
       </c>
     </row>
-    <row r="26" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2030</v>
       </c>
@@ -6513,7 +6571,7 @@
         <v>1347.756592</v>
       </c>
     </row>
-    <row r="27" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2029</v>
       </c>
@@ -6617,7 +6675,7 @@
         <v>1325.5010990000001</v>
       </c>
     </row>
-    <row r="28" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2028</v>
       </c>
@@ -6721,7 +6779,7 @@
         <v>1300.290283</v>
       </c>
     </row>
-    <row r="29" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2027</v>
       </c>
@@ -6825,7 +6883,7 @@
         <v>1262.6137699999999</v>
       </c>
     </row>
-    <row r="30" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2026</v>
       </c>
@@ -6929,7 +6987,7 @@
         <v>1227.352539</v>
       </c>
     </row>
-    <row r="31" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2025</v>
       </c>
@@ -7033,7 +7091,7 @@
         <v>1195.4132079999999</v>
       </c>
     </row>
-    <row r="32" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2024</v>
       </c>
@@ -7137,7 +7195,7 @@
         <v>1181.6953120000001</v>
       </c>
     </row>
-    <row r="33" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2023</v>
       </c>
@@ -7241,7 +7299,7 @@
         <v>1141.3917240000001</v>
       </c>
     </row>
-    <row r="34" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2022</v>
       </c>
@@ -7345,7 +7403,7 @@
         <v>1120.0336910000001</v>
       </c>
     </row>
-    <row r="35" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2021</v>
       </c>
@@ -7449,7 +7507,7 @@
         <v>1091.1320800000001</v>
       </c>
     </row>
-    <row r="36" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2020</v>
       </c>
@@ -7553,7 +7611,7 @@
         <v>1062.568481</v>
       </c>
     </row>
-    <row r="37" spans="1:34" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:34" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2019</v>
       </c>
@@ -7564,7 +7622,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AF46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -7574,19 +7632,19 @@
       <selection pane="bottomRight" activeCell="A48" sqref="A48:XFD60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.59765625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="10.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.6328125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>2020</v>
       </c>
@@ -7681,12 +7739,12 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -7784,7 +7842,7 @@
         <v>1.3531296060545272E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -7882,7 +7940,7 @@
         <v>2.3350238322795862E-6</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -7980,12 +8038,12 @@
         <v>6.1053021960695644E-7</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -8083,7 +8141,7 @@
         <v>9.8726194433162944E-8</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>64</v>
       </c>
@@ -8181,7 +8239,7 @@
         <v>1.7036654570280245E-7</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -8279,12 +8337,12 @@
         <v>4.4545123318962488E-8</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -8413,7 +8471,7 @@
         <v>1.45185580048769E-6</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -8542,7 +8600,7 @@
         <v>2.5053903779823887E-6</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>24</v>
       </c>
@@ -8671,12 +8729,12 @@
         <v>6.5507534292591893E-7</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>2020</v>
       </c>
@@ -8771,12 +8829,12 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -8874,7 +8932,7 @@
         <v>1.483504698310363E-6</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>64</v>
       </c>
@@ -8972,7 +9030,7 @@
         <v>3.2257406405890635E-6</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>24</v>
       </c>
@@ -9070,12 +9128,12 @@
         <v>6.1053021960695655E-7</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="26" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -9173,7 +9231,7 @@
         <v>1.0823854022006941E-7</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>64</v>
       </c>
@@ -9271,7 +9329,7 @@
         <v>2.3535446733911626E-7</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>24</v>
       </c>
@@ -9369,12 +9427,12 @@
         <v>4.4545123318962501E-8</v>
       </c>
     </row>
-    <row r="30" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="31" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -9503,7 +9561,7 @@
         <v>1.5917432385304324E-6</v>
       </c>
     </row>
-    <row r="32" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -9632,7 +9690,7 @@
         <v>3.4610951079281799E-6</v>
       </c>
     </row>
-    <row r="33" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -9761,12 +9819,12 @@
         <v>6.5507534292591904E-7</v>
       </c>
     </row>
-    <row r="35" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -9895,7 +9953,7 @@
         <v>1.3988743804274244E-7</v>
       </c>
     </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>64</v>
       </c>
@@ -10024,7 +10082,7 @@
         <v>9.5570472994579118E-7</v>
       </c>
     </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -10153,12 +10211,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>22</v>
       </c>
@@ -10279,7 +10337,7 @@
         <v>9.4295244364286254E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>64</v>
       </c>
@@ -10400,12 +10458,12 @@
         <v>0.29627451070315025</v>
       </c>
     </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>22</v>
       </c>
@@ -10526,7 +10584,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>64</v>
       </c>
@@ -10653,24 +10711,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AF29"/>
   <sheetViews>
     <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="45" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>2020</v>
       </c>
@@ -10765,7 +10823,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -10894,7 +10952,7 @@
         <v>73.266311999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -11023,12 +11081,12 @@
         <v>41.961776999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -11126,7 +11184,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>164</v>
       </c>
@@ -11224,7 +11282,7 @@
         <v>78.485100000000003</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>165</v>
       </c>
@@ -11322,7 +11380,7 @@
         <v>394.678</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>166</v>
       </c>
@@ -11420,7 +11478,7 @@
         <v>45.619</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>167</v>
       </c>
@@ -11518,7 +11576,7 @@
         <v>79.558999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>168</v>
       </c>
@@ -11616,7 +11674,7 @@
         <v>424.64400000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>169</v>
       </c>
@@ -11714,7 +11772,7 @@
         <v>766.69899999999996</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>170</v>
       </c>
@@ -11812,7 +11870,7 @@
         <v>2.5379999999999998</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>171</v>
       </c>
@@ -11910,7 +11968,7 @@
         <v>1.0999999999999999E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>172</v>
       </c>
@@ -12008,7 +12066,7 @@
         <v>5.8259999999999996</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>173</v>
       </c>
@@ -12106,7 +12164,7 @@
         <v>25.167999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>174</v>
       </c>
@@ -12204,7 +12262,7 @@
         <v>205.69499999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>175</v>
       </c>
@@ -12302,7 +12360,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>176</v>
       </c>
@@ -12400,7 +12458,7 @@
         <v>54.939</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>177</v>
       </c>
@@ -12498,7 +12556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>178</v>
       </c>
@@ -12596,7 +12654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>179</v>
       </c>
@@ -12694,7 +12752,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>180</v>
       </c>
@@ -12823,12 +12881,12 @@
         <v>78.575100000000006</v>
       </c>
     </row>
-    <row r="27" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="28" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -12836,7 +12894,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="29" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>24</v>
       </c>
@@ -12851,24 +12909,24 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AJ119"/>
   <sheetViews>
     <sheetView topLeftCell="A99" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="A102" sqref="A102"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="68.59765625" customWidth="1"/>
-    <col min="2" max="2" width="39.73046875" customWidth="1"/>
+    <col min="1" max="1" width="68.6328125" customWidth="1"/>
+    <col min="2" max="2" width="39.7265625" customWidth="1"/>
     <col min="3" max="3" width="31" customWidth="1"/>
-    <col min="4" max="4" width="27.86328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.73046875" bestFit="1" customWidth="1"/>
-    <col min="6" max="36" width="11.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="27.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.7265625" bestFit="1" customWidth="1"/>
+    <col min="6" max="36" width="11.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>58</v>
       </c>
@@ -12908,7 +12966,7 @@
       <c r="AI1" s="10"/>
       <c r="AJ1" s="10"/>
     </row>
-    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>41</v>
       </c>
@@ -12922,7 +12980,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>117</v>
       </c>
@@ -12930,7 +12988,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
         <v>120</v>
       </c>
@@ -12941,7 +12999,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="5" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>50</v>
       </c>
@@ -12952,7 +13010,7 @@
         <v>3.6256791591385165</v>
       </c>
     </row>
-    <row r="6" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -12963,7 +13021,7 @@
         <v>3.5973528438891544</v>
       </c>
     </row>
-    <row r="7" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>24</v>
       </c>
@@ -12974,7 +13032,7 @@
         <v>0.15230684857126578</v>
       </c>
     </row>
-    <row r="8" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>25</v>
       </c>
@@ -12985,7 +13043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>48</v>
       </c>
@@ -12996,7 +13054,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -13007,7 +13065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>28</v>
       </c>
@@ -13018,7 +13076,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -13029,7 +13087,7 @@
         <v>6.9518421539183022</v>
       </c>
     </row>
-    <row r="13" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>30</v>
       </c>
@@ -13040,7 +13098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -13051,7 +13109,7 @@
         <v>2.2124867557274697</v>
       </c>
     </row>
-    <row r="15" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>32</v>
       </c>
@@ -13062,7 +13120,7 @@
         <v>7.295618081459569</v>
       </c>
     </row>
-    <row r="16" spans="1:36" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:36" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>47</v>
       </c>
@@ -13073,7 +13131,7 @@
         <v>6.1423270460699575</v>
       </c>
     </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -13084,7 +13142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -13095,7 +13153,7 @@
         <v>2.2124867557274697</v>
       </c>
     </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>52</v>
       </c>
@@ -13106,7 +13164,7 @@
         <v>2.2124867557274697</v>
       </c>
     </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>53</v>
       </c>
@@ -13117,12 +13175,12 @@
         <v>6.7522876908857299</v>
       </c>
     </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>2020</v>
       </c>
@@ -13217,7 +13275,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>40</v>
       </c>
@@ -13315,7 +13373,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A26" s="7" t="s">
         <v>69</v>
       </c>
@@ -13414,7 +13472,7 @@
       </c>
       <c r="AG26" s="7"/>
     </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A27" s="7" t="s">
         <v>70</v>
       </c>
@@ -13513,7 +13571,7 @@
       </c>
       <c r="AG27" s="7"/>
     </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A28" s="7" t="s">
         <v>71</v>
       </c>
@@ -13612,7 +13670,7 @@
       </c>
       <c r="AG28" s="7"/>
     </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A29" s="7" t="s">
         <v>72</v>
       </c>
@@ -13711,7 +13769,7 @@
       </c>
       <c r="AG29" s="7"/>
     </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A30" s="7" t="s">
         <v>73</v>
       </c>
@@ -13810,7 +13868,7 @@
       </c>
       <c r="AG30" s="7"/>
     </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A31" s="7" t="s">
         <v>74</v>
       </c>
@@ -13909,7 +13967,7 @@
       </c>
       <c r="AG31" s="7"/>
     </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A32" s="7" t="s">
         <v>75</v>
       </c>
@@ -14008,7 +14066,7 @@
       </c>
       <c r="AG32" s="7"/>
     </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A33" s="7" t="s">
         <v>76</v>
       </c>
@@ -14107,7 +14165,7 @@
       </c>
       <c r="AG33" s="7"/>
     </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A34" s="7" t="s">
         <v>77</v>
       </c>
@@ -14206,7 +14264,7 @@
       </c>
       <c r="AG34" s="7"/>
     </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A35" s="7" t="s">
         <v>78</v>
       </c>
@@ -14305,7 +14363,7 @@
       </c>
       <c r="AG35" s="7"/>
     </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A36" s="7" t="s">
         <v>79</v>
       </c>
@@ -14404,7 +14462,7 @@
       </c>
       <c r="AG36" s="7"/>
     </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A37" s="7" t="s">
         <v>80</v>
       </c>
@@ -14503,7 +14561,7 @@
       </c>
       <c r="AG37" s="7"/>
     </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A38" s="7" t="s">
         <v>81</v>
       </c>
@@ -14602,7 +14660,7 @@
       </c>
       <c r="AG38" s="7"/>
     </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A39" s="7" t="s">
         <v>82</v>
       </c>
@@ -14701,7 +14759,7 @@
       </c>
       <c r="AG39" s="7"/>
     </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A40" s="7" t="s">
         <v>83</v>
       </c>
@@ -14800,7 +14858,7 @@
       </c>
       <c r="AG40" s="7"/>
     </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A41" s="7" t="s">
         <v>84</v>
       </c>
@@ -14899,12 +14957,12 @@
       </c>
       <c r="AG41" s="7"/>
     </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.35">
       <c r="B44">
         <v>2019</v>
       </c>
@@ -14999,7 +15057,7 @@
         <v>2049</v>
       </c>
     </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>40</v>
       </c>
@@ -15097,7 +15155,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A47" s="7" t="s">
         <v>85</v>
       </c>
@@ -15196,7 +15254,7 @@
       </c>
       <c r="AG47" s="7"/>
     </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A48" s="7" t="s">
         <v>86</v>
       </c>
@@ -15295,7 +15353,7 @@
       </c>
       <c r="AG48" s="7"/>
     </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A49" s="7" t="s">
         <v>87</v>
       </c>
@@ -15394,7 +15452,7 @@
       </c>
       <c r="AG49" s="7"/>
     </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>88</v>
       </c>
@@ -15492,7 +15550,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>89</v>
       </c>
@@ -15590,7 +15648,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>90</v>
       </c>
@@ -15688,7 +15746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>91</v>
       </c>
@@ -15786,7 +15844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A54" s="7" t="s">
         <v>92</v>
       </c>
@@ -15885,7 +15943,7 @@
       </c>
       <c r="AG54" s="7"/>
     </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>93</v>
       </c>
@@ -15983,7 +16041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A56" s="7" t="s">
         <v>94</v>
       </c>
@@ -16082,7 +16140,7 @@
       </c>
       <c r="AG56" s="7"/>
     </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A57" s="7" t="s">
         <v>95</v>
       </c>
@@ -16181,7 +16239,7 @@
       </c>
       <c r="AG57" s="7"/>
     </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A58" s="7" t="s">
         <v>96</v>
       </c>
@@ -16280,7 +16338,7 @@
       </c>
       <c r="AG58" s="7"/>
     </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>97</v>
       </c>
@@ -16378,7 +16436,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A60" s="7" t="s">
         <v>98</v>
       </c>
@@ -16477,7 +16535,7 @@
       </c>
       <c r="AG60" s="7"/>
     </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A61" s="7" t="s">
         <v>99</v>
       </c>
@@ -16576,7 +16634,7 @@
       </c>
       <c r="AG61" s="7"/>
     </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A62" s="7" t="s">
         <v>100</v>
       </c>
@@ -16675,12 +16733,12 @@
       </c>
       <c r="AG62" s="7"/>
     </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="66" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>40</v>
       </c>
@@ -16778,7 +16836,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="67" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>101</v>
       </c>
@@ -16876,7 +16934,7 @@
         <v>0.496</v>
       </c>
     </row>
-    <row r="68" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>102</v>
       </c>
@@ -16974,7 +17032,7 @@
         <v>0.55000000000000004</v>
       </c>
     </row>
-    <row r="69" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>103</v>
       </c>
@@ -17072,7 +17130,7 @@
         <v>0.92500000000000004</v>
       </c>
     </row>
-    <row r="70" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>104</v>
       </c>
@@ -17170,7 +17228,7 @@
         <v>0.41899999999999998</v>
       </c>
     </row>
-    <row r="71" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>105</v>
       </c>
@@ -17268,7 +17326,7 @@
         <v>0.32411699999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>106</v>
       </c>
@@ -17366,7 +17424,7 @@
         <v>0.18706500000000001</v>
       </c>
     </row>
-    <row r="73" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>107</v>
       </c>
@@ -17464,7 +17522,7 @@
         <v>0.23599999999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>108</v>
       </c>
@@ -17562,7 +17620,7 @@
         <v>0.61799999999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>109</v>
       </c>
@@ -17660,7 +17718,7 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="76" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>110</v>
       </c>
@@ -17758,7 +17816,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>111</v>
       </c>
@@ -17856,7 +17914,7 @@
         <v>0.125</v>
       </c>
     </row>
-    <row r="78" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>112</v>
       </c>
@@ -17954,7 +18012,7 @@
         <v>0.376</v>
       </c>
     </row>
-    <row r="79" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>113</v>
       </c>
@@ -18052,7 +18110,7 @@
         <v>0.480263</v>
       </c>
     </row>
-    <row r="80" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>114</v>
       </c>
@@ -18150,7 +18208,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="81" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>115</v>
       </c>
@@ -18248,7 +18306,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="82" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>116</v>
       </c>
@@ -18346,12 +18404,12 @@
         <v>0.65400000000000003</v>
       </c>
     </row>
-    <row r="84" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="85" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>22</v>
       </c>
@@ -18360,7 +18418,7 @@
         <v>26.066283669753769</v>
       </c>
     </row>
-    <row r="86" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>23</v>
       </c>
@@ -18369,7 +18427,7 @@
         <v>21.782138646809884</v>
       </c>
     </row>
-    <row r="87" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>24</v>
       </c>
@@ -18378,7 +18436,7 @@
         <v>25.753337773875877</v>
       </c>
     </row>
-    <row r="88" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>25</v>
       </c>
@@ -18387,7 +18445,7 @@
         <v>4.2262119900023958</v>
       </c>
     </row>
-    <row r="89" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>26</v>
       </c>
@@ -18396,7 +18454,7 @@
         <v>11.730636715120365</v>
       </c>
     </row>
-    <row r="90" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>56</v>
       </c>
@@ -18405,7 +18463,7 @@
         <v>14.157752989132563</v>
       </c>
     </row>
-    <row r="91" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>57</v>
       </c>
@@ -18414,7 +18472,7 @@
         <v>37.250973918973365</v>
       </c>
     </row>
-    <row r="92" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>29</v>
       </c>
@@ -18423,7 +18481,7 @@
         <v>51.692042559319695</v>
       </c>
     </row>
-    <row r="93" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>30</v>
       </c>
@@ -18432,7 +18490,7 @@
         <v>16.578278466908674</v>
       </c>
     </row>
-    <row r="94" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>31</v>
       </c>
@@ -18441,7 +18499,7 @@
         <v>202.57269797690168</v>
       </c>
     </row>
-    <row r="95" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>32</v>
       </c>
@@ -18450,7 +18508,7 @@
         <v>33.363908971946358</v>
       </c>
     </row>
-    <row r="96" spans="1:32" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>47</v>
       </c>
@@ -18459,7 +18517,7 @@
         <v>29.467737117179439</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>49</v>
       </c>
@@ -18468,7 +18526,7 @@
         <v>20.276644647381922</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>51</v>
       </c>
@@ -18477,7 +18535,7 @@
         <v>76.314880896901684</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>52</v>
       </c>
@@ -18486,7 +18544,7 @@
         <v>108.78307897690168</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>53</v>
       </c>
@@ -18495,12 +18553,12 @@
         <v>51.04414633518396</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A102" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>22</v>
       </c>
@@ -18511,7 +18569,7 @@
       <c r="C103" s="8"/>
       <c r="D103" s="14"/>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>23</v>
       </c>
@@ -18522,7 +18580,7 @@
       <c r="C104" s="8"/>
       <c r="D104" s="14"/>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>24</v>
       </c>
@@ -18533,7 +18591,7 @@
       <c r="C105" s="8"/>
       <c r="D105" s="14"/>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>25</v>
       </c>
@@ -18544,7 +18602,7 @@
       <c r="C106" s="8"/>
       <c r="D106" s="14"/>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>26</v>
       </c>
@@ -18555,7 +18613,7 @@
       <c r="C107" s="8"/>
       <c r="D107" s="14"/>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>56</v>
       </c>
@@ -18566,7 +18624,7 @@
       <c r="C108" s="8"/>
       <c r="D108" s="14"/>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>57</v>
       </c>
@@ -18577,7 +18635,7 @@
       <c r="C109" s="8"/>
       <c r="D109" s="14"/>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>29</v>
       </c>
@@ -18588,7 +18646,7 @@
       <c r="C110" s="8"/>
       <c r="D110" s="14"/>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>30</v>
       </c>
@@ -18599,7 +18657,7 @@
       <c r="C111" s="8"/>
       <c r="D111" s="14"/>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>31</v>
       </c>
@@ -18610,7 +18668,7 @@
       <c r="C112" s="8"/>
       <c r="D112" s="14"/>
     </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>32</v>
       </c>
@@ -18621,7 +18679,7 @@
       <c r="C113" s="8"/>
       <c r="D113" s="14"/>
     </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>47</v>
       </c>
@@ -18632,7 +18690,7 @@
       <c r="C114" s="8"/>
       <c r="D114" s="14"/>
     </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>49</v>
       </c>
@@ -18643,7 +18701,7 @@
       <c r="C115" s="8"/>
       <c r="D115" s="14"/>
     </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>51</v>
       </c>
@@ -18654,7 +18712,7 @@
       <c r="C116" s="8"/>
       <c r="D116" s="14"/>
     </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>52</v>
       </c>
@@ -18665,7 +18723,7 @@
       <c r="C117" s="8"/>
       <c r="D117" s="14"/>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>53</v>
       </c>
@@ -18676,7 +18734,7 @@
       <c r="C118" s="8"/>
       <c r="D118" s="14"/>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D119" s="14"/>
     </row>
   </sheetData>
@@ -18689,108 +18747,99 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.1328125" customWidth="1"/>
+    <col min="1" max="1" width="27.08984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>50</v>
       </c>
       <c r="B2" s="4">
-        <f>'High OGS Calibration'!B28</f>
-        <v>5000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="4">
-        <f>$B$2*Weighting!B104</f>
-        <v>4178.2209774853654</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
       <c r="B4" s="4">
-        <f>'High OGS Calibration'!B29</f>
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
       <c r="B5" s="4">
-        <f>$B$2*Weighting!B106</f>
-        <v>810.66638488752358</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>48</v>
       </c>
       <c r="B6" s="4">
-        <f>$B$2*Weighting!B107</f>
-        <v>2250.1551935330367</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="4">
-        <f>$B$2*Weighting!B108</f>
-        <v>2715.7214216847929</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>28</v>
       </c>
       <c r="B8" s="4">
-        <f>$B$2*Weighting!B109</f>
-        <v>7145.432465733089</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>29</v>
       </c>
       <c r="B9" s="4">
-        <f>$B$2*Weighting!B110</f>
-        <v>9915.499120287137</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="4">
-        <f>$B$2*Weighting!B111</f>
-        <v>3180.0234120342629</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" s="5" t="s">
         <v>31</v>
       </c>
@@ -18798,7 +18847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>32</v>
       </c>
@@ -18806,25 +18855,23 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="4">
-        <f>$B$2*Weighting!B114</f>
-        <v>5652.4622939196688</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>49</v>
       </c>
       <c r="B14" s="4">
-        <f>$B$2*Weighting!B115</f>
-        <v>3889.4391130466547</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -18832,7 +18879,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -18840,13 +18887,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>53</v>
       </c>
       <c r="B17" s="4">
-        <f>$B$2*Weighting!B118</f>
-        <v>9791.2205249291947</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>